<commit_message>
Add some validation for operands passed to the CF Wizards  - remove any leading ``=` from formulae, because they'll be embedded into other formulae  - unwrap any string literals from quotes, because that's also handled internally
Handle cross-worksheet cell references in cellReferences and Formulae/Expressions

Basic Xlsx reading of CF Rules/Styles from <extLst><ext><ConditinalFormattings> element, and not just the <ConditinalFormatting> element of the worksheet
</commit_message>
<xml_diff>
--- a/tests/data/Style/ConditionalFormatting/CellMatcher.xlsx
+++ b/tests/data/Style/ConditionalFormatting/CellMatcher.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\PHPOffice\PHPSpreadsheet\develop\tests\data\Style\ConditionalFormatting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86D1AF2B-4C08-47F6-8B0A-3E2F0A1B76FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7342C8C3-7883-40DA-A5EB-F712D0F5F9A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1474" yWindow="1474" windowWidth="24686" windowHeight="16723" activeTab="1" xr2:uid="{C11EA5FA-62FC-4B18-BE9C-0527028CF0E2}"/>
+    <workbookView xWindow="1440" yWindow="1440" windowWidth="24686" windowHeight="16723" xr2:uid="{C11EA5FA-62FC-4B18-BE9C-0527028CF0E2}"/>
   </bookViews>
   <sheets>
     <sheet name="cellIs Comparison" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,9 @@
     <sheet name="Blank Expressions" sheetId="5" r:id="rId5"/>
     <sheet name="Error Expressions" sheetId="6" r:id="rId6"/>
     <sheet name="Date Expressions" sheetId="7" r:id="rId7"/>
+    <sheet name="Duplicates Expressions" sheetId="13" r:id="rId8"/>
+    <sheet name="CrossSheet References" sheetId="11" r:id="rId9"/>
+    <sheet name="CrossSheet Values" sheetId="12" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="70">
   <si>
     <t>HELLO</t>
   </si>
@@ -103,18 +106,6 @@
     <t>SLEEPY</t>
   </si>
   <si>
-    <t>Text Begins With</t>
-  </si>
-  <si>
-    <t>Text Ends With</t>
-  </si>
-  <si>
-    <t>Text Contains</t>
-  </si>
-  <si>
-    <t>Text Doesn't Contain</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -155,6 +146,114 @@
   </si>
   <si>
     <t>NEXT MONTH</t>
+  </si>
+  <si>
+    <t>Contains Literal</t>
+  </si>
+  <si>
+    <t>Doesn't Contain Literal</t>
+  </si>
+  <si>
+    <t>Begins with CellRef</t>
+  </si>
+  <si>
+    <t>Ends with CellRef</t>
+  </si>
+  <si>
+    <t>Contains CellRef</t>
+  </si>
+  <si>
+    <t>Doesn't Contain CellRef</t>
+  </si>
+  <si>
+    <t>Begins with Formula</t>
+  </si>
+  <si>
+    <t>Ends with Formula</t>
+  </si>
+  <si>
+    <t>Contains Formula</t>
+  </si>
+  <si>
+    <t>Doesn't Contain Formula</t>
+  </si>
+  <si>
+    <t>Ends with Literal</t>
+  </si>
+  <si>
+    <t>Begins with Literal</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>ISODD()/ISEVEN() Formula</t>
+  </si>
+  <si>
+    <t>Sales Grid for Country</t>
+  </si>
+  <si>
+    <t>Sales Grid for Country and Quarter</t>
+  </si>
+  <si>
+    <t>Value between Literals</t>
+  </si>
+  <si>
+    <t>Value Between Cell References</t>
+  </si>
+  <si>
+    <t>Value Between with Formula</t>
+  </si>
+  <si>
+    <t>Value Between with Unordered Cell References</t>
+  </si>
+  <si>
+    <t>(where Quarter value could be mistaken for a cell reference)</t>
+  </si>
+  <si>
+    <t>Compare Text with Formula</t>
+  </si>
+  <si>
+    <t>Less than/Equal/Greater than with Cell Reference</t>
+  </si>
+  <si>
+    <t>Less than/Equal/Greater than with Literal</t>
+  </si>
+  <si>
+    <t>Blank/Not Blank</t>
+  </si>
+  <si>
+    <t>Error/Not Error</t>
+  </si>
+  <si>
+    <t>Duplicates/Unique</t>
+  </si>
+  <si>
+    <t>Compare Text with Cell Reference containing Formula</t>
+  </si>
+  <si>
+    <t>HE</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>WOR</t>
+  </si>
+  <si>
+    <t>LO</t>
+  </si>
+  <si>
+    <t>Compare Cell Greater/Less with Vertical Cell Reference</t>
   </si>
 </sst>
 </file>
@@ -164,7 +263,7 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="&quot;£&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yyyy"/>
-    <numFmt numFmtId="167" formatCode="dd\-mmm\ hh:mm"/>
+    <numFmt numFmtId="166" formatCode="dd\-mmm\ hh:mm"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -212,19 +311,43 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="47">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -395,7 +518,63 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -464,6 +643,27 @@
       <font>
         <color rgb="FF006100"/>
       </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.59996337778862885"/>
@@ -838,97 +1038,107 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9A1847-4841-41F6-B579-FB898076071D}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
-      <c r="A1" s="1">
-        <v>-3</v>
-      </c>
-      <c r="B1" s="1">
-        <v>-2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B2" s="1">
         <v>-2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>-1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
       <c r="E2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="1">
         <v>-1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
       <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
       <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.4">
@@ -1019,7 +1229,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1031,32 +1246,134 @@
         <v>HELLO</v>
       </c>
     </row>
+    <row r="23" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>65</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+      <c r="E24" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" t="s">
+        <v>48</v>
+      </c>
+      <c r="E25" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A33">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A34">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A37">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:E5">
-    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThan">
+  <conditionalFormatting sqref="A2:E6">
+    <cfRule type="cellIs" dxfId="46" priority="8" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10:E14 G10">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="5" operator="greaterThan">
       <formula>$G$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="6" operator="equal">
       <formula>$G$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="7" operator="lessThan">
       <formula>$G$10</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:C20">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="4" operator="equal">
       <formula>"HELLO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:B25">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="equal">
+      <formula>_xlfn.CONCAT($C24,$D24,$E24)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A30:A37">
+    <cfRule type="cellIs" dxfId="38" priority="1" operator="greaterThan">
+      <formula>$A29</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="2" operator="lessThan">
+      <formula>$A29</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1064,12 +1381,52 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECED6FA7-3406-4873-8E48-AC92F7F1FA30}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7793DDEF-4D6D-4821-9D89-8A5D80E983D8}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1077,73 +1434,77 @@
     <col min="1" max="1" width="11.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1">
-        <v>-2</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A2">
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A3">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A10">
-        <v>2</v>
-      </c>
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>6</v>
+    <row r="10" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A12">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A13">
         <v>4</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>3</v>
       </c>
-      <c r="C12">
+      <c r="C13">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A16">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>3</v>
-      </c>
-      <c r="C16">
-        <v>7</v>
+    <row r="16" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
@@ -1151,51 +1512,67 @@
         <v>5</v>
       </c>
       <c r="B17">
+        <v>3</v>
+      </c>
+      <c r="C17">
         <v>7</v>
       </c>
-      <c r="C17">
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>5</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A21" s="6">
-        <f ca="1">TODAY()-0.5</f>
-        <v>44571.5</v>
+    <row r="21" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="6">
-        <f ca="1">TODAY()+0.5</f>
-        <v>44572.5</v>
+        <f ca="1">TODAY()-0.5</f>
+        <v>44579.5</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="6">
+        <f ca="1">TODAY()+0.5</f>
+        <v>44580.5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A24" s="6">
         <f ca="1">TODAY()+1.5</f>
-        <v>44573.5</v>
+        <v>44581.5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A5">
-    <cfRule type="cellIs" dxfId="25" priority="4" operator="between">
+  <conditionalFormatting sqref="A2:A6">
+    <cfRule type="cellIs" dxfId="36" priority="4" operator="between">
       <formula>-1</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A10:A12">
-    <cfRule type="cellIs" dxfId="24" priority="3" operator="between">
-      <formula>$B10</formula>
-      <formula>$C10</formula>
+  <conditionalFormatting sqref="A11:A13">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="between">
+      <formula>$B11</formula>
+      <formula>$C11</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A16:A17">
-    <cfRule type="cellIs" dxfId="23" priority="2" operator="between">
-      <formula>$B16</formula>
-      <formula>$C16</formula>
+  <conditionalFormatting sqref="A17:A18">
+    <cfRule type="cellIs" dxfId="34" priority="2" operator="between">
+      <formula>$B17</formula>
+      <formula>$C17</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:A23">
-    <cfRule type="cellIs" dxfId="22" priority="1" operator="between">
+  <conditionalFormatting sqref="A22:A24">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="between">
       <formula>TODAY()</formula>
       <formula>TODAY()+1</formula>
     </cfRule>
@@ -1207,312 +1584,330 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A77248-E1F9-414F-9064-70E68DF206CE}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A1" s="1">
-        <v>-3</v>
-      </c>
-      <c r="B1" s="1">
-        <v>-2</v>
-      </c>
-      <c r="C1" s="1">
-        <v>-1</v>
-      </c>
-      <c r="D1" s="1">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1">
-        <v>1</v>
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" s="1">
+        <v>-3</v>
+      </c>
+      <c r="B2" s="1">
         <v>-2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>-1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
-        <v>1</v>
-      </c>
       <c r="E2" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" s="1">
+        <v>-2</v>
+      </c>
+      <c r="B3" s="1">
         <v>-1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>0</v>
       </c>
-      <c r="C3" s="1">
-        <v>1</v>
-      </c>
       <c r="D3" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
         <v>2</v>
-      </c>
-      <c r="E3" s="1">
-        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" s="1">
+        <v>-1</v>
+      </c>
+      <c r="B4" s="1">
         <v>0</v>
       </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
       <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
-      <c r="D4" s="1">
+      <c r="E4" s="1">
         <v>3</v>
-      </c>
-      <c r="E4" s="1">
-        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
         <v>2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>3</v>
       </c>
-      <c r="D5" s="1">
+      <c r="E5" s="1">
         <v>4</v>
       </c>
-      <c r="E5" s="1">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2">
-        <v>16753</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B12" s="2">
-        <v>14808</v>
+        <v>16753</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D12" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
-        <v>10644</v>
+        <v>14808</v>
       </c>
       <c r="C13" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>1390</v>
+        <v>10644</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2">
-        <v>4865</v>
+        <v>1390</v>
       </c>
       <c r="C15" t="s">
         <v>10</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2">
+        <v>4865</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B17" s="2">
         <v>12438</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>7</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>6</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B22" s="2">
         <v>16753</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>7</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" t="s">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A23" t="s">
         <v>9</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B23" s="2">
         <v>14808</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C23" t="s">
         <v>10</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" t="s">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A24" t="s">
         <v>12</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B24" s="2">
         <v>10644</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" t="s">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B25" s="2">
         <v>1390</v>
-      </c>
-      <c r="C24" t="s">
-        <v>10</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B25" s="2">
-        <v>4865</v>
       </c>
       <c r="C25" t="s">
         <v>10</v>
       </c>
       <c r="D25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4865</v>
+      </c>
+      <c r="C26" t="s">
+        <v>10</v>
+      </c>
+      <c r="D26" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A27" t="s">
         <v>12</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B27" s="2">
         <v>12438</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>7</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A11:D16">
-    <cfRule type="expression" dxfId="21" priority="4">
-      <formula>$C11="USA"</formula>
+  <conditionalFormatting sqref="A12:D17 A20">
+    <cfRule type="expression" dxfId="32" priority="4">
+      <formula>$C12="USA"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:D26">
-    <cfRule type="expression" dxfId="20" priority="3">
-      <formula>AND($C21="USA",$D21="Q4")</formula>
+  <conditionalFormatting sqref="A22:D27">
+    <cfRule type="expression" dxfId="31" priority="3">
+      <formula>AND($C22="USA",$D22="Q4")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:E5">
-    <cfRule type="expression" dxfId="19" priority="1">
-      <formula>ISEVEN(A1)</formula>
+  <conditionalFormatting sqref="A2:E6">
+    <cfRule type="expression" dxfId="30" priority="1">
+      <formula>ISEVEN(A2)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="2">
-      <formula>ISODD(A1)</formula>
+    <cfRule type="expression" dxfId="29" priority="2">
+      <formula>ISODD(A2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1522,158 +1917,372 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27F5215F-DA12-4A53-B99F-DA348E75720D}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="3" max="3" width="9.23046875" style="7"/>
+    <col min="9" max="10" width="9.23046875" style="7"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+      <c r="H2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A3" t="s">
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7" s="7"/>
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
         <v>0</v>
       </c>
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="F6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
+      <c r="D8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
         <v>19</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A11" t="s">
+      <c r="D10" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="7"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A14" t="s">
         <v>0</v>
       </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A12" t="s">
+      <c r="D14" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="J14" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B15" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A13" t="s">
+      <c r="D15" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A16" t="s">
         <v>19</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B16" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
-      <c r="A16" t="s">
+      <c r="D16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="7"/>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A20" t="s">
         <v>0</v>
       </c>
-      <c r="B16" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="F16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A17" t="s">
+      <c r="D20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" t="s">
+        <v>1</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A21" t="s">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B21" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A18" t="s">
+      <c r="D21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A22" t="s">
         <v>19</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B22" t="s">
         <v>18</v>
       </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" t="s">
+        <v>19</v>
+      </c>
+      <c r="H22" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:B4">
+    <cfRule type="beginsWith" dxfId="28" priority="14" operator="beginsWith" text="H">
+      <formula>LEFT(A2,LEN("H"))="H"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A8:B10">
+    <cfRule type="endsWith" dxfId="27" priority="13" operator="endsWith" text="OW">
+      <formula>RIGHT(A8,LEN("OW"))="OW"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A14:B16">
+    <cfRule type="containsText" dxfId="26" priority="12" operator="containsText" text="LL">
+      <formula>NOT(ISERROR(SEARCH("LL",A14)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="beginsWith" priority="6" operator="beginsWith" id="{74583FC1-E418-46A3-B42E-189388009748}">
-            <xm:f>LEFT(A1,LEN($F$1))=$F$1</xm:f>
-            <xm:f>$F$1</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="7" tint="0.59996337778862885"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A1:B3</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="endsWith" priority="5" operator="endsWith" id="{BF15D19F-31D8-446A-A485-646B0ACC6F9C}">
-            <xm:f>RIGHT(A6,LEN($F$6))=$F$6</xm:f>
-            <xm:f>$F$6</xm:f>
+          <x14:cfRule type="notContainsText" priority="11" operator="notContains" id="{2E660F70-A841-4AA9-BAD4-986F6E749CA0}">
+            <xm:f>ISERROR(SEARCH($C$20,A20))</xm:f>
+            <xm:f>$C$20</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1682,12 +2291,12 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A6:B8</xm:sqref>
+          <xm:sqref>A20:B22</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{A101C484-B831-4153-B441-5A0CC13105B7}">
-            <xm:f>NOT(ISERROR(SEARCH($F$11,A11)))</xm:f>
-            <xm:f>$F$11</xm:f>
+          <x14:cfRule type="beginsWith" priority="8" operator="beginsWith" id="{9AB19EC2-499B-4A2C-9F88-4FF4C36F26DF}">
+            <xm:f>LEFT(D2,LEN($C$2))=$C$2</xm:f>
+            <xm:f>$C$2</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1696,12 +2305,12 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A11:B13</xm:sqref>
+          <xm:sqref>D2:E4</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="notContainsText" priority="3" operator="notContains" id="{2E660F70-A841-4AA9-BAD4-986F6E749CA0}">
-            <xm:f>ISERROR(SEARCH($F$16,A16))</xm:f>
-            <xm:f>$F$16</xm:f>
+          <x14:cfRule type="endsWith" priority="7" operator="endsWith" id="{3431114E-8055-4687-9C35-5A60068A2DEC}">
+            <xm:f>RIGHT(D8,LEN($C$8))=$C$8</xm:f>
+            <xm:f>$C$8</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill>
@@ -1710,7 +2319,91 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A16:B18</xm:sqref>
+          <xm:sqref>D8:E10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{76D39A3F-6928-43A5-B44A-29329A7CFC14}">
+            <xm:f>NOT(ISERROR(SEARCH($C$14,D14)))</xm:f>
+            <xm:f>$C$14</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D14:E16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="notContainsText" priority="5" operator="notContains" id="{5A7AA221-7A1C-4B8E-8B32-36312462C31D}">
+            <xm:f>ISERROR(SEARCH($C$20,D20))</xm:f>
+            <xm:f>$C$20</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>D20:E22</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{0E778EC3-E535-41E4-9E33-3443E3CAA51F}">
+            <xm:f>NOT(ISERROR(SEARCH(_xlfn.CONCAT($I$2,$J$2),G2)))</xm:f>
+            <xm:f>_xlfn.CONCAT($I$2,$J$2)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G2:H4</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="endsWith" priority="3" operator="endsWith" id="{1849D206-CD17-44EE-B991-9972EB8AEA69}">
+            <xm:f>RIGHT(G8,LEN(_xlfn.CONCAT($I$8,$J$8)))=_xlfn.CONCAT($I$8,$J$8)</xm:f>
+            <xm:f>_xlfn.CONCAT($I$8,$J$8)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G8:H10</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{5EA6DB2B-9C4C-45E1-8961-F9572A57A7D5}">
+            <xm:f>NOT(ISERROR(SEARCH(_xlfn.CONCAT($I$14,$J$14),G14)))</xm:f>
+            <xm:f>_xlfn.CONCAT($I$14,$J$14)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G14:H16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="notContainsText" priority="1" operator="notContains" id="{AD6BF2E0-FD19-4C56-B96E-8507573D9D52}">
+            <xm:f>ISERROR(SEARCH(_xlfn.CONCAT($I$20,$J$20),G20))</xm:f>
+            <xm:f>_xlfn.CONCAT($I$20,$J$20)</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="7" tint="0.39994506668294322"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G20:H22</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -1720,31 +2413,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB0B7264-345F-4B0D-9293-AB934074F713}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
-      <c r="B2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:B2">
-    <cfRule type="containsBlanks" dxfId="13" priority="3">
-      <formula>LEN(TRIM(A1))=0</formula>
+  <conditionalFormatting sqref="A2:B3">
+    <cfRule type="containsBlanks" dxfId="16" priority="3">
+      <formula>LEN(TRIM(A2))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="12" priority="4">
-      <formula>LEN(TRIM(A1))&gt;0</formula>
+    <cfRule type="notContainsBlanks" dxfId="15" priority="4">
+      <formula>LEN(TRIM(A2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1753,24 +2451,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FC539E8-892F-4D9F-941A-551328934F29}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A1">
-        <v>5</v>
-      </c>
-      <c r="B1">
-        <v>-2</v>
-      </c>
-      <c r="C1">
-        <f>A1/B1</f>
-        <v>-2.5</v>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -1778,11 +2469,11 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="C2">
         <f>A2/B2</f>
-        <v>-5</v>
+        <v>-2.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -1790,11 +2481,11 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="e">
+        <v>-1</v>
+      </c>
+      <c r="C3">
         <f>A3/B3</f>
-        <v>#DIV/0!</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -1802,11 +2493,11 @@
         <v>5</v>
       </c>
       <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="C4" t="e">
         <f>A4/B4</f>
-        <v>5</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -1814,20 +2505,32 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5">
         <f>A5/B5</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>A6/B6</f>
         <v>2.5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C1:C5">
-    <cfRule type="containsErrors" dxfId="11" priority="3">
-      <formula>ISERROR(C1)</formula>
+  <conditionalFormatting sqref="C2:C6">
+    <cfRule type="containsErrors" dxfId="14" priority="3">
+      <formula>ISERROR(C2)</formula>
     </cfRule>
-    <cfRule type="notContainsErrors" dxfId="10" priority="4">
-      <formula>NOT(ISERROR(C1))</formula>
+    <cfRule type="notContainsErrors" dxfId="13" priority="4">
+      <formula>NOT(ISERROR(C2))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1836,10 +2539,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0704E190-C724-4693-848D-88BACF397F2A}">
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1853,34 +2556,34 @@
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.4">
@@ -1888,772 +2591,1033 @@
         <v>-365</v>
       </c>
       <c r="B2" s="3">
-        <f t="shared" ref="B2:K2" ca="1" si="0">TODAY()+$A2</f>
-        <v>44207</v>
+        <f t="shared" ref="B2:K3" ca="1" si="0">TODAY()+$A2</f>
+        <v>44215</v>
       </c>
       <c r="C2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="D2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="E2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="F2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="G2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="H2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="I2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="J2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
       <c r="K2" s="3">
         <f t="shared" ca="1" si="0"/>
-        <v>44207</v>
+        <v>44215</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3">
+        <v>-35</v>
+      </c>
+      <c r="B3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="C3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="D3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="E3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="F3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="G3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="H3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="I3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="J3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+      <c r="K3" s="3">
+        <f t="shared" ca="1" si="0"/>
+        <v>44545</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A4">
         <v>-28</v>
       </c>
-      <c r="B3" s="3">
-        <f t="shared" ref="B3:K17" ca="1" si="1">TODAY()+$A3</f>
-        <v>44544</v>
-      </c>
-      <c r="C3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="D3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="E3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="F3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="G3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="H3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="I3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="J3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-      <c r="K3" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44544</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
-      <c r="A4">
-        <v>-14</v>
-      </c>
       <c r="B4" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <f t="shared" ref="B4:K19" ca="1" si="1">TODAY()+$A4</f>
+        <v>44552</v>
       </c>
       <c r="C4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="E4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="F4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="G4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="H4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="I4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="J4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
       <c r="K4" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44558</v>
+        <v>44552</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5">
-        <v>-8</v>
+        <v>-14</v>
       </c>
       <c r="B5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="E5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="F5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="G5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="I5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="J5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
       <c r="K5" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44564</v>
+        <v>44566</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="B6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="C6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="E6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="F6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="G6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="H6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="I6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="J6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
       <c r="K6" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44565</v>
+        <v>44572</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7">
-        <v>-2</v>
+        <v>-7</v>
       </c>
       <c r="B7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="E7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="F7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="G7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="H7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="I7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="J7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
       <c r="K7" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44570</v>
+        <v>44573</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="B8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="E8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="F8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="G8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="I8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="J8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
       <c r="K8" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44571</v>
+        <v>44578</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="E9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="F9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="G9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="I9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="J9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
       <c r="K9" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44572</v>
+        <v>44579</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="C10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="E10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="F10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="G10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="I10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="J10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
       <c r="K10" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44573</v>
+        <v>44580</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="C11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="E11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="F11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="G11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="I11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="J11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
       <c r="K11" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44574</v>
+        <v>44581</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="C12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="D12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="E12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="F12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="G12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="I12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="J12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44576</v>
+        <v>44582</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="C13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="D13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="E13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="F13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="G13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="H13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="I13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="J13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
       <c r="K13" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44579</v>
+        <v>44584</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="C14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="D14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="E14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="F14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="G14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="H14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="I14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="J14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44580</v>
+        <v>44587</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="C15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="D15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="E15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="F15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="G15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="H15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="I15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="J15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
       <c r="K15" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44586</v>
+        <v>44588</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A16">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="C16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="D16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="E16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="F16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="G16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="H16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="I16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="J16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
       <c r="K16" s="3">
         <f t="shared" ca="1" si="1"/>
-        <v>44600</v>
+        <v>44594</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A17">
+        <v>28</v>
+      </c>
+      <c r="B17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="D17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="E17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="G17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="H17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="J17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A18">
+        <v>35</v>
+      </c>
+      <c r="B18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="C18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="D18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="E18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="G18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="H18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="J18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+      <c r="K18" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44615</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="A19">
         <v>365</v>
       </c>
-      <c r="B17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="C17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="D17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="F17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="G17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="I17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="J17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
-      </c>
-      <c r="K17" s="3">
-        <f t="shared" ca="1" si="1"/>
-        <v>44937</v>
+      <c r="B19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="E19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
+      </c>
+      <c r="K19" s="3">
+        <f t="shared" ca="1" si="1"/>
+        <v>44945</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:B17">
-    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="today">
+  <conditionalFormatting sqref="B2:B19">
+    <cfRule type="timePeriod" dxfId="12" priority="10" timePeriod="today">
       <formula>FLOOR(B2,1)=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C2:C17">
-    <cfRule type="timePeriod" dxfId="8" priority="9" timePeriod="yesterday">
+  <conditionalFormatting sqref="C2:C19">
+    <cfRule type="timePeriod" dxfId="11" priority="9" timePeriod="yesterday">
       <formula>FLOOR(C2,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D17">
-    <cfRule type="timePeriod" dxfId="7" priority="8" timePeriod="tomorrow">
+  <conditionalFormatting sqref="D2:D19">
+    <cfRule type="timePeriod" dxfId="10" priority="8" timePeriod="tomorrow">
       <formula>FLOOR(D2,1)=TODAY()+1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E17">
-    <cfRule type="timePeriod" dxfId="6" priority="7" timePeriod="last7Days">
+  <conditionalFormatting sqref="E2:E19">
+    <cfRule type="timePeriod" dxfId="9" priority="7" timePeriod="last7Days">
       <formula>AND(TODAY()-FLOOR(E2,1)&lt;=6,FLOOR(E2,1)&lt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F17">
-    <cfRule type="timePeriod" dxfId="5" priority="6" timePeriod="lastWeek">
+  <conditionalFormatting sqref="F2:F19">
+    <cfRule type="timePeriod" dxfId="8" priority="6" timePeriod="lastWeek">
       <formula>AND(TODAY()-ROUNDDOWN(F2,0)&gt;=(WEEKDAY(TODAY())),TODAY()-ROUNDDOWN(F2,0)&lt;(WEEKDAY(TODAY())+7))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G2:G17">
-    <cfRule type="timePeriod" dxfId="4" priority="5" timePeriod="thisWeek">
+  <conditionalFormatting sqref="G2:G19">
+    <cfRule type="timePeriod" dxfId="7" priority="5" timePeriod="thisWeek">
       <formula>AND(TODAY()-ROUNDDOWN(G2,0)&lt;=WEEKDAY(TODAY())-1,ROUNDDOWN(G2,0)-TODAY()&lt;=7-WEEKDAY(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H17">
-    <cfRule type="timePeriod" dxfId="3" priority="4" timePeriod="nextWeek">
+  <conditionalFormatting sqref="H2:H19">
+    <cfRule type="timePeriod" dxfId="6" priority="4" timePeriod="nextWeek">
       <formula>AND(ROUNDDOWN(H2,0)-TODAY()&gt;(7-WEEKDAY(TODAY())),ROUNDDOWN(H2,0)-TODAY()&lt;(15-WEEKDAY(TODAY())))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I17">
-    <cfRule type="timePeriod" dxfId="2" priority="3" timePeriod="lastMonth">
+  <conditionalFormatting sqref="I2:I19">
+    <cfRule type="timePeriod" dxfId="5" priority="3" timePeriod="lastMonth">
       <formula>AND(MONTH(I2)=MONTH(EDATE(TODAY(),0-1)),YEAR(I2)=YEAR(EDATE(TODAY(),0-1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J17">
-    <cfRule type="timePeriod" dxfId="1" priority="2" timePeriod="thisMonth">
+  <conditionalFormatting sqref="J2:J19">
+    <cfRule type="timePeriod" dxfId="4" priority="2" timePeriod="thisMonth">
       <formula>AND(MONTH(J2)=MONTH(TODAY()),YEAR(J2)=YEAR(TODAY()))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K17">
-    <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="nextMonth">
+  <conditionalFormatting sqref="K2:K19">
+    <cfRule type="timePeriod" dxfId="3" priority="1" timePeriod="nextMonth">
       <formula>AND(MONTH(K2)=MONTH(EDATE(TODAY(),0+1)),YEAR(K2)=YEAR(EDATE(TODAY(),0+1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB5BFE97-55E5-4709-B65F-DF956819CBEC}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <f>B2+B3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <f t="shared" ref="B5:B11" si="0">B3+B4</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:B11">
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="uniqueValues" dxfId="1" priority="2"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6114D7EC-809E-43D6-B72E-A5743871B36D}">
+  <dimension ref="A1:A5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.4">
+      <c r="A5">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{BE102189-172C-496F-9829-AF5BE1563708}">
+            <xm:f>'CrossSheet Values'!$A1</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor theme="9" tint="0.59996337778862885"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A1:A5</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>